<commit_message>
complete homework X-1-1 :)
</commit_message>
<xml_diff>
--- a/Stage X/X-1 Database. Basics/X-1-1 Homework/Tabs.xlsx
+++ b/Stage X/X-1 Database. Basics/X-1-1 Homework/Tabs.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gamer-PC\Desktop\GB-Git\Stage X\X-1-1 Database Homework\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gamer-PC\Desktop\GB-Git\Stage X\X-1 Database. Basics\X-1-1 Homework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DAFC68D-EEE3-4C81-82BB-8EC000A41970}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F05F1A96-4F30-42F1-BC1B-931C6AB245CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="53">
   <si>
     <t>Преподаватель</t>
   </si>
@@ -147,25 +147,43 @@
     <t>Ключ курса</t>
   </si>
   <si>
-    <t>Наименование курса</t>
-  </si>
-  <si>
     <t>Потоки</t>
   </si>
   <si>
     <t>Ключ потока</t>
   </si>
   <si>
-    <t>Ключ учеников</t>
-  </si>
-  <si>
-    <t>Ученики</t>
-  </si>
-  <si>
     <t>Успеваемость</t>
   </si>
   <si>
-    <t>Дата начала обуч.</t>
+    <t>Имя курса</t>
+  </si>
+  <si>
+    <t>Дата начала</t>
+  </si>
+  <si>
+    <t>Поток</t>
+  </si>
+  <si>
+    <t>Пользователи</t>
+  </si>
+  <si>
+    <t>Ключ пользователя</t>
+  </si>
+  <si>
+    <t>Соцсети</t>
+  </si>
+  <si>
+    <t>Instagramm</t>
+  </si>
+  <si>
+    <t>VK</t>
+  </si>
+  <si>
+    <t>Рейтинг</t>
+  </si>
+  <si>
+    <t>Соцсеть</t>
   </si>
 </sst>
 </file>
@@ -201,15 +219,27 @@
       <charset val="204"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -232,35 +262,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -280,22 +286,25 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -361,6 +370,106 @@
         <charset val="204"/>
         <scheme val="none"/>
       </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Rosatom"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Rosatom"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Rosatom"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Rosatom"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Rosatom"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="none"/>
+      </font>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -381,167 +490,27 @@
         <charset val="204"/>
         <scheme val="none"/>
       </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Rosatom"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="none"/>
+      </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Rosatom"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Rosatom"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Rosatom"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Rosatom"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Rosatom"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Rosatom"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Rosatom"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Rosatom"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -683,6 +652,46 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Rosatom"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Rosatom"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -698,33 +707,33 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{19AF1261-AD67-4E36-A3AC-427EBC689198}" name="Таблица3" displayName="Таблица3" ref="B3:H8" totalsRowShown="0" headerRowDxfId="1" dataDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{19AF1261-AD67-4E36-A3AC-427EBC689198}" name="Таблица3" displayName="Таблица3" ref="B3:H8" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
   <autoFilter ref="B3:H8" xr:uid="{19AF1261-AD67-4E36-A3AC-427EBC689198}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{38D79A2E-9280-4895-8457-F7BB01C3E74F}" name="Преподаватель" dataDxfId="18"/>
-    <tableColumn id="2" xr3:uid="{B9D43D6E-B544-4897-A23B-5E02C856AFF5}" name="Электронная почта" dataDxfId="17"/>
-    <tableColumn id="3" xr3:uid="{AC0F8660-B644-4E15-9BAB-AFADE14BF018}" name="Курс" dataDxfId="16"/>
-    <tableColumn id="4" xr3:uid="{7B562F93-C4A8-479C-A8E4-33859632A4A6}" name="Номер потока" dataDxfId="15"/>
-    <tableColumn id="5" xr3:uid="{4CF11B6E-E613-490E-B9CA-D3DEC25A2D7A}" name="Дата начала обучения" dataDxfId="14"/>
-    <tableColumn id="6" xr3:uid="{F3D1E964-49EA-4B79-9233-86E29417238A}" name="Количество учеников" dataDxfId="13"/>
-    <tableColumn id="7" xr3:uid="{0DC5F2D5-7905-480E-B2FB-D743B403F11D}" name="Успеваемость учеников" dataDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{38D79A2E-9280-4895-8457-F7BB01C3E74F}" name="Преподаватель" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{B9D43D6E-B544-4897-A23B-5E02C856AFF5}" name="Электронная почта" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{AC0F8660-B644-4E15-9BAB-AFADE14BF018}" name="Курс" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{7B562F93-C4A8-479C-A8E4-33859632A4A6}" name="Номер потока" dataDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{4CF11B6E-E613-490E-B9CA-D3DEC25A2D7A}" name="Дата начала обучения" dataDxfId="12"/>
+    <tableColumn id="6" xr3:uid="{F3D1E964-49EA-4B79-9233-86E29417238A}" name="Количество учеников" dataDxfId="11"/>
+    <tableColumn id="7" xr3:uid="{0DC5F2D5-7905-480E-B2FB-D743B403F11D}" name="Успеваемость учеников" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{7B794C34-18F3-4027-B4F9-2D607B40C25C}" name="Таблица5" displayName="Таблица5" ref="J3:Q7" totalsRowShown="0" headerRowDxfId="0" dataDxfId="2">
-  <autoFilter ref="J3:Q7" xr:uid="{7B794C34-18F3-4027-B4F9-2D607B40C25C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{7B794C34-18F3-4027-B4F9-2D607B40C25C}" name="Таблица5" displayName="Таблица5" ref="B21:I25" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="B21:I25" xr:uid="{7B794C34-18F3-4027-B4F9-2D607B40C25C}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{860D316D-1755-42C9-82B4-7EBFF43BBCD4}" name="Пользователь" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{7435A26B-ECD7-4223-8E7A-814179E3F731}" name="Возраст" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{24C37496-0160-42D0-9CCA-641664A1CA6F}" name="Instagram" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{16DE8E91-3D92-40A3-8FAA-3903CBD5CBD3}" name="Facebook" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{7E3E13EA-B043-48D2-A8EC-394CC8CC815F}" name="TikTok" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{03583A4B-4CB6-45B1-B51C-D0FD52F1672A}" name="YouTube" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{71AC0146-D3FC-47FE-8DC2-6CC34FFB2EED}" name="Twitter" dataDxfId="4"/>
-    <tableColumn id="8" xr3:uid="{5AC18D73-C103-45D8-9AD9-4EDA976C44E1}" name="Вконтакте" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{860D316D-1755-42C9-82B4-7EBFF43BBCD4}" name="Пользователь" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{7435A26B-ECD7-4223-8E7A-814179E3F731}" name="Возраст" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{24C37496-0160-42D0-9CCA-641664A1CA6F}" name="Instagram" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{16DE8E91-3D92-40A3-8FAA-3903CBD5CBD3}" name="Facebook" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{7E3E13EA-B043-48D2-A8EC-394CC8CC815F}" name="TikTok" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{03583A4B-4CB6-45B1-B51C-D0FD52F1672A}" name="YouTube" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{71AC0146-D3FC-47FE-8DC2-6CC34FFB2EED}" name="Twitter" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{5AC18D73-C103-45D8-9AD9-4EDA976C44E1}" name="Вконтакте" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -993,60 +1002,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:Q15"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="B1:Q34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="I34" sqref="B1:I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.7109375" style="6" customWidth="1"/>
     <col min="2" max="8" width="15.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="3.7109375" style="2" customWidth="1"/>
-    <col min="10" max="17" width="15.7109375" style="9" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" style="2" customWidth="1"/>
+    <col min="10" max="10" width="3.7109375" style="8" customWidth="1"/>
+    <col min="11" max="17" width="15.7109375" style="8" customWidth="1"/>
     <col min="18" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="7" t="s">
+    <row r="1" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="J1" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7"/>
-      <c r="Q1" s="7"/>
-    </row>
-    <row r="2" spans="2:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
-      <c r="O2" s="7"/>
-      <c r="P2" s="7"/>
-      <c r="Q2" s="7"/>
-    </row>
-    <row r="3" spans="2:17" s="1" customFormat="1" ht="27" x14ac:dyDescent="0.25">
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+    </row>
+    <row r="2" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+    </row>
+    <row r="3" spans="2:8" s="1" customFormat="1" ht="27" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1068,36 +1063,12 @@
       <c r="H3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q3" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="2:17" ht="27" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="2:8" ht="27" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="7" t="s">
         <v>16</v>
       </c>
       <c r="D4" s="3" t="s">
@@ -1115,36 +1086,12 @@
       <c r="H4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="J4" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="K4" s="1">
-        <v>23</v>
-      </c>
-      <c r="L4" s="1">
-        <v>1</v>
-      </c>
-      <c r="M4" s="1">
-        <v>2</v>
-      </c>
-      <c r="N4" s="1">
-        <v>3</v>
-      </c>
-      <c r="O4" s="1">
-        <v>1</v>
-      </c>
-      <c r="P4" s="1">
-        <v>4</v>
-      </c>
-      <c r="Q4" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="2:17" ht="27" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="2:8" ht="27" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="7" t="s">
         <v>17</v>
       </c>
       <c r="D5" s="3" t="s">
@@ -1162,36 +1109,12 @@
       <c r="H5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="J5" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="K5" s="1">
-        <v>16</v>
-      </c>
-      <c r="L5" s="1">
-        <v>1</v>
-      </c>
-      <c r="M5" s="1">
-        <v>3</v>
-      </c>
-      <c r="N5" s="1">
-        <v>1</v>
-      </c>
-      <c r="O5" s="1">
-        <v>2</v>
-      </c>
-      <c r="P5" s="1">
-        <v>4</v>
-      </c>
-      <c r="Q5" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="2:17" ht="27" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="2:8" ht="27" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="7" t="s">
         <v>18</v>
       </c>
       <c r="D6" s="3" t="s">
@@ -1209,32 +1132,8 @@
       <c r="H6" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="J6" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="K6" s="1">
-        <v>34</v>
-      </c>
-      <c r="L6" s="1">
-        <v>2</v>
-      </c>
-      <c r="M6" s="1">
-        <v>1</v>
-      </c>
-      <c r="N6" s="1">
-        <v>4</v>
-      </c>
-      <c r="O6" s="1">
-        <v>3</v>
-      </c>
-      <c r="P6" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q6" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="2:17" ht="27" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="2:8" ht="27" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>7</v>
       </c>
@@ -1256,36 +1155,12 @@
       <c r="H7" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="J7" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="K7" s="1">
-        <v>25</v>
-      </c>
-      <c r="L7" s="1">
-        <v>4</v>
-      </c>
-      <c r="M7" s="1">
-        <v>1</v>
-      </c>
-      <c r="N7" s="1">
-        <v>1</v>
-      </c>
-      <c r="O7" s="1">
-        <v>2</v>
-      </c>
-      <c r="P7" s="1">
-        <v>4</v>
-      </c>
-      <c r="Q7" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="2:17" ht="27" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="2:8" ht="27" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="7" t="s">
         <v>17</v>
       </c>
       <c r="D8" s="3" t="s">
@@ -1304,81 +1179,373 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B9" s="9"/>
-    </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="8"/>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="12" t="s">
         <v>33</v>
       </c>
       <c r="D11" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="F11" s="12" t="s">
+      <c r="E11" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="H11" s="12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" ht="27" x14ac:dyDescent="0.25">
+      <c r="B12" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B14" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="11"/>
+      <c r="E14" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B15" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" s="11"/>
+      <c r="E15" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="H11" s="12" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="12" spans="2:17" ht="27" x14ac:dyDescent="0.25">
-      <c r="B12" s="10" t="s">
+    </row>
+    <row r="16" spans="2:8" ht="27" x14ac:dyDescent="0.25">
+      <c r="D16" s="11"/>
+      <c r="E16" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D17" s="11"/>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B18" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B20" s="10"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
+    </row>
+    <row r="21" spans="2:9" ht="67.5" x14ac:dyDescent="0.25">
+      <c r="B21" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" ht="27" x14ac:dyDescent="0.25">
+      <c r="B22" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" s="1">
+        <v>23</v>
+      </c>
+      <c r="D22" s="1">
+        <v>1</v>
+      </c>
+      <c r="E22" s="1">
+        <v>2</v>
+      </c>
+      <c r="F22" s="1">
+        <v>3</v>
+      </c>
+      <c r="G22" s="1">
+        <v>1</v>
+      </c>
+      <c r="H22" s="1">
+        <v>4</v>
+      </c>
+      <c r="I22" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" ht="27" x14ac:dyDescent="0.25">
+      <c r="B23" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23" s="1">
+        <v>16</v>
+      </c>
+      <c r="D23" s="1">
+        <v>1</v>
+      </c>
+      <c r="E23" s="1">
+        <v>3</v>
+      </c>
+      <c r="F23" s="1">
+        <v>1</v>
+      </c>
+      <c r="G23" s="1">
+        <v>2</v>
+      </c>
+      <c r="H23" s="1">
+        <v>4</v>
+      </c>
+      <c r="I23" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B24" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" s="1">
         <v>34</v>
       </c>
-      <c r="D12" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="H12" s="10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="13" spans="2:17" ht="27" x14ac:dyDescent="0.25">
-      <c r="B13" s="10" t="s">
+      <c r="D24" s="1">
+        <v>2</v>
+      </c>
+      <c r="E24" s="1">
+        <v>1</v>
+      </c>
+      <c r="F24" s="1">
+        <v>4</v>
+      </c>
+      <c r="G24" s="1">
+        <v>3</v>
+      </c>
+      <c r="H24" s="1">
+        <v>1</v>
+      </c>
+      <c r="I24" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" ht="27" x14ac:dyDescent="0.25">
+      <c r="B25" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25" s="1">
+        <v>25</v>
+      </c>
+      <c r="D25" s="1">
+        <v>4</v>
+      </c>
+      <c r="E25" s="1">
+        <v>1</v>
+      </c>
+      <c r="F25" s="1">
+        <v>1</v>
+      </c>
+      <c r="G25" s="1">
+        <v>2</v>
+      </c>
+      <c r="H25" s="1">
+        <v>4</v>
+      </c>
+      <c r="I25" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="8"/>
+      <c r="I26" s="8"/>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B27" s="8"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="8"/>
+      <c r="I27" s="8"/>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B28" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C28" s="8"/>
+      <c r="D28" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="E28" s="8"/>
+      <c r="F28" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="G28" s="8"/>
+      <c r="H28" s="8"/>
+      <c r="I28" s="8"/>
+    </row>
+    <row r="29" spans="2:9" ht="27" x14ac:dyDescent="0.25">
+      <c r="B29" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C29" s="8"/>
+      <c r="D29" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E29" s="8"/>
+      <c r="F29" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G29" s="8"/>
+      <c r="H29" s="8"/>
+      <c r="I29" s="8"/>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B30" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C30" s="8"/>
+      <c r="D30" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E30" s="8"/>
+      <c r="F30" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="G30" s="8"/>
+      <c r="H30" s="8"/>
+      <c r="I30" s="8"/>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B31" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="D13" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="F13" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="H13" s="11" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="14" spans="2:17" ht="27" x14ac:dyDescent="0.25">
-      <c r="B14" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="F14" s="10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B15" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="F15" s="11" t="s">
-        <v>45</v>
-      </c>
+      <c r="C31" s="8"/>
+      <c r="D31" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E31" s="8"/>
+      <c r="F31" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="G31" s="8"/>
+      <c r="H31" s="8"/>
+      <c r="I31" s="8"/>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B32" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C32" s="8"/>
+      <c r="D32" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E32" s="8"/>
+      <c r="F32" s="8"/>
+      <c r="G32" s="8"/>
+      <c r="H32" s="8"/>
+      <c r="I32" s="8"/>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B33" s="8"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E33" s="8"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="8"/>
+      <c r="H33" s="8"/>
+      <c r="I33" s="8"/>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B34" s="8"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="E34" s="8"/>
+      <c r="F34" s="8"/>
+      <c r="G34" s="8"/>
+      <c r="H34" s="8"/>
+      <c r="I34" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="J1:Q2"/>
+    <mergeCell ref="B18:I20"/>
     <mergeCell ref="B1:H2"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.19685039370078741" bottom="0.19685039370078741" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" scale="77" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
   <tableParts count="2">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>

</xml_diff>